<commit_message>
seteo fecha actual pago
</commit_message>
<xml_diff>
--- a/Excel/Esqueletos Excel/esqueletoVenta.xlsx
+++ b/Excel/Esqueletos Excel/esqueletoVenta.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>cliente:</t>
   </si>
@@ -28,7 +28,10 @@
     <t>fecha:</t>
   </si>
   <si>
-    <t>pagó:</t>
+    <t>Pagó (Si, No):</t>
+  </si>
+  <si>
+    <t>si</t>
   </si>
   <si>
     <t>codigo articulo</t>
@@ -60,6 +63,7 @@
   <fonts count="5">
     <font>
       <name val="Arial"/>
+      <charset val="1"/>
       <family val="2"/>
       <sz val="10"/>
     </font>
@@ -80,6 +84,7 @@
     </font>
     <font>
       <name val="Arial"/>
+      <charset val="1"/>
       <family val="2"/>
       <color rgb="00800000"/>
       <sz val="16"/>
@@ -151,14 +156,14 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="86" zoomScaleNormal="86" zoomScalePageLayoutView="100">
-      <selection activeCell="B1" activeCellId="0" pane="topLeft" sqref="B1"/>
+      <selection activeCell="B3" activeCellId="0" pane="topLeft" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.4313725490196"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.7803921568627"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.2980392156863"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.5764705882353"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.6392156862745"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.1254901960784"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.6235294117647"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.6941176470588"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="19.3" outlineLevel="0" r="1">
@@ -172,31 +177,31 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="n">
-        <v>41667</v>
+        <v>41992</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="19.3" outlineLevel="0" r="2">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="0" t="n">
-        <v>139.55</v>
+      <c r="B2" s="0" t="s">
+        <v>4</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="22.55" outlineLevel="0" r="3">
       <c r="A3" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="4">
       <c r="A4" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>5</v>
@@ -207,7 +212,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="5">
       <c r="A5" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>1</v>
@@ -218,7 +223,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="6">
       <c r="A6" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>10</v>
@@ -245,17 +250,17 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60">
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5764705882353"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6941176470588"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -270,17 +275,17 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60">
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5764705882353"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6941176470588"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>